<commit_message>
update results for bv_cutoff min_percent compare
</commit_message>
<xml_diff>
--- a/Material-coord/softBV-coord_mix.xlsx
+++ b/Material-coord/softBV-coord_mix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\softBV_mix\GitHub\projects\Coord\Material-coord\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Github\Projects\Coord\Material-coord\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77FA7E60-E58F-4B2C-9442-1D31B21DE38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD128745-A418-4D89-9C9F-249E335FC387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -473,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -482,6 +482,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,16 +824,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I141" sqref="I141"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101:F101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -851,7 +853,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -868,13 +870,13 @@
         <v>3</v>
       </c>
       <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G2" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -893,11 +895,11 @@
       <c r="F3">
         <v>4</v>
       </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -914,13 +916,13 @@
         <v>-1</v>
       </c>
       <c r="F4">
-        <v>6</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -937,13 +939,13 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -960,13 +962,13 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G6" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -985,11 +987,11 @@
       <c r="F7">
         <v>4</v>
       </c>
-      <c r="G7">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1006,13 +1008,13 @@
         <v>-2</v>
       </c>
       <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G8" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1029,13 +1031,13 @@
         <v>-1</v>
       </c>
       <c r="F9">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G9" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1052,13 +1054,13 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G10" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1075,13 +1077,13 @@
         <v>-2</v>
       </c>
       <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G11" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1100,11 +1102,11 @@
       <c r="F12">
         <v>3</v>
       </c>
-      <c r="G12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G12" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1123,11 +1125,11 @@
       <c r="F13">
         <v>3</v>
       </c>
-      <c r="G13">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G13" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1144,13 +1146,13 @@
         <v>4</v>
       </c>
       <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G14" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1167,13 +1169,13 @@
         <v>-2</v>
       </c>
       <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G15" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1190,13 +1192,13 @@
         <v>4</v>
       </c>
       <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G16" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1213,13 +1215,13 @@
         <v>-2</v>
       </c>
       <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G17" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1238,11 +1240,11 @@
       <c r="F18">
         <v>4</v>
       </c>
-      <c r="G18">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1261,11 +1263,11 @@
       <c r="F19">
         <v>4</v>
       </c>
-      <c r="G19">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1282,13 +1284,13 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G20" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1307,11 +1309,11 @@
       <c r="F21">
         <v>4</v>
       </c>
-      <c r="G21">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1328,13 +1330,13 @@
         <v>2</v>
       </c>
       <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1351,13 +1353,13 @@
         <v>-2</v>
       </c>
       <c r="F23">
-        <v>2</v>
-      </c>
-      <c r="G23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1374,13 +1376,13 @@
         <v>-2</v>
       </c>
       <c r="F24">
-        <v>3</v>
-      </c>
-      <c r="G24">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G24" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1399,11 +1401,11 @@
       <c r="F25">
         <v>4</v>
       </c>
-      <c r="G25">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1420,13 +1422,13 @@
         <v>2</v>
       </c>
       <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G26" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1445,11 +1447,11 @@
       <c r="F27">
         <v>3</v>
       </c>
-      <c r="G27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1468,11 +1470,11 @@
       <c r="F28">
         <v>3</v>
       </c>
-      <c r="G28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1491,11 +1493,11 @@
       <c r="F29">
         <v>3</v>
       </c>
-      <c r="G29">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1514,11 +1516,11 @@
       <c r="F30">
         <v>3</v>
       </c>
-      <c r="G30">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1537,11 +1539,11 @@
       <c r="F31">
         <v>3</v>
       </c>
-      <c r="G31">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1558,13 +1560,13 @@
         <v>2</v>
       </c>
       <c r="F32">
-        <v>6</v>
-      </c>
-      <c r="G32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1581,13 +1583,13 @@
         <v>-2</v>
       </c>
       <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1604,13 +1606,13 @@
         <v>-2</v>
       </c>
       <c r="F34">
-        <v>2</v>
-      </c>
-      <c r="G34" s="2">
+        <v>3</v>
+      </c>
+      <c r="G34" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1627,13 +1629,13 @@
         <v>2</v>
       </c>
       <c r="F35">
-        <v>7</v>
-      </c>
-      <c r="G35">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1650,13 +1652,13 @@
         <v>3</v>
       </c>
       <c r="F36">
-        <v>5</v>
-      </c>
-      <c r="G36">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G36" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1673,13 +1675,13 @@
         <v>3</v>
       </c>
       <c r="F37">
-        <v>5</v>
-      </c>
-      <c r="G37">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G37" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1696,13 +1698,13 @@
         <v>-2</v>
       </c>
       <c r="F38">
-        <v>4</v>
-      </c>
-      <c r="G38">
         <v>5</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1719,13 +1721,13 @@
         <v>-2</v>
       </c>
       <c r="F39">
-        <v>4</v>
-      </c>
-      <c r="G39">
         <v>5</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1742,13 +1744,13 @@
         <v>-2</v>
       </c>
       <c r="F40">
-        <v>4</v>
-      </c>
-      <c r="G40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1765,13 +1767,13 @@
         <v>-2</v>
       </c>
       <c r="F41">
-        <v>4</v>
-      </c>
-      <c r="G41">
         <v>5</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1788,13 +1790,13 @@
         <v>2</v>
       </c>
       <c r="F42">
-        <v>1</v>
-      </c>
-      <c r="G42">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G42" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1811,13 +1813,13 @@
         <v>2</v>
       </c>
       <c r="F43">
-        <v>5</v>
-      </c>
-      <c r="G43">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G43" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1834,13 +1836,13 @@
         <v>-2</v>
       </c>
       <c r="F44">
-        <v>1</v>
-      </c>
-      <c r="G44">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G44" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1857,13 +1859,13 @@
         <v>-2</v>
       </c>
       <c r="F45">
-        <v>3</v>
-      </c>
-      <c r="G45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G45" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1880,13 +1882,13 @@
         <v>-2</v>
       </c>
       <c r="F46">
-        <v>1</v>
-      </c>
-      <c r="G46">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G46" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1905,11 +1907,11 @@
       <c r="F47">
         <v>4</v>
       </c>
-      <c r="G47">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1926,13 +1928,13 @@
         <v>-1</v>
       </c>
       <c r="F48">
-        <v>4</v>
-      </c>
-      <c r="G48">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G48" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1949,13 +1951,13 @@
         <v>-1</v>
       </c>
       <c r="F49">
-        <v>1</v>
-      </c>
-      <c r="G49">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G49" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1972,13 +1974,13 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>7</v>
-      </c>
-      <c r="G50">
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1995,13 +1997,13 @@
         <v>2</v>
       </c>
       <c r="F51">
-        <v>5</v>
-      </c>
-      <c r="G51">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G51" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2018,13 +2020,13 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>8</v>
-      </c>
-      <c r="G52">
         <v>11</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2041,13 +2043,13 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>6</v>
-      </c>
-      <c r="G53">
         <v>9</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2066,11 +2068,11 @@
       <c r="F54">
         <v>1</v>
       </c>
-      <c r="G54" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2087,13 +2089,13 @@
         <v>-2</v>
       </c>
       <c r="F55">
-        <v>2</v>
-      </c>
-      <c r="G55" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G55" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2110,13 +2112,13 @@
         <v>-2</v>
       </c>
       <c r="F56">
-        <v>1</v>
-      </c>
-      <c r="G56" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G56" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2135,11 +2137,11 @@
       <c r="F57">
         <v>4</v>
       </c>
-      <c r="G57">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2156,13 +2158,13 @@
         <v>3</v>
       </c>
       <c r="F58">
-        <v>5</v>
-      </c>
-      <c r="G58">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G58" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2181,11 +2183,11 @@
       <c r="F59">
         <v>4</v>
       </c>
-      <c r="G59">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2204,11 +2206,11 @@
       <c r="F60">
         <v>4</v>
       </c>
-      <c r="G60">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G60" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2225,13 +2227,13 @@
         <v>1</v>
       </c>
       <c r="F61">
-        <v>5</v>
-      </c>
-      <c r="G61">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G61" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2248,13 +2250,13 @@
         <v>-2</v>
       </c>
       <c r="F62">
-        <v>1</v>
-      </c>
-      <c r="G62" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G62" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2273,11 +2275,11 @@
       <c r="F63">
         <v>4</v>
       </c>
-      <c r="G63">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G63" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2294,13 +2296,13 @@
         <v>-2</v>
       </c>
       <c r="F64">
-        <v>1</v>
-      </c>
-      <c r="G64">
         <v>5</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G64" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2317,13 +2319,13 @@
         <v>-2</v>
       </c>
       <c r="F65">
-        <v>1</v>
-      </c>
-      <c r="G65">
         <v>5</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G65" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2340,13 +2342,13 @@
         <v>4</v>
       </c>
       <c r="F66">
-        <v>5</v>
-      </c>
-      <c r="G66">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G66" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2363,13 +2365,13 @@
         <v>2</v>
       </c>
       <c r="F67">
-        <v>5</v>
-      </c>
-      <c r="G67">
         <v>7</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G67" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2386,13 +2388,13 @@
         <v>2</v>
       </c>
       <c r="F68">
-        <v>9</v>
-      </c>
-      <c r="G68">
         <v>12</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2409,13 +2411,13 @@
         <v>-2</v>
       </c>
       <c r="F69">
-        <v>4</v>
-      </c>
-      <c r="G69">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G69" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2432,13 +2434,13 @@
         <v>-2</v>
       </c>
       <c r="F70">
-        <v>1</v>
-      </c>
-      <c r="G70">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G70" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2455,13 +2457,13 @@
         <v>4</v>
       </c>
       <c r="F71">
-        <v>5</v>
-      </c>
-      <c r="G71">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G71" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2480,11 +2482,11 @@
       <c r="F72">
         <v>3</v>
       </c>
-      <c r="G72">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G72" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2501,13 +2503,13 @@
         <v>2</v>
       </c>
       <c r="F73">
-        <v>1</v>
-      </c>
-      <c r="G73">
         <v>9</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2524,13 +2526,13 @@
         <v>-2</v>
       </c>
       <c r="F74">
-        <v>2</v>
-      </c>
-      <c r="G74">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G74" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2547,13 +2549,13 @@
         <v>-2</v>
       </c>
       <c r="F75">
-        <v>1</v>
-      </c>
-      <c r="G75">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G75" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2570,13 +2572,13 @@
         <v>4</v>
       </c>
       <c r="F76">
-        <v>1</v>
-      </c>
-      <c r="G76">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G76" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2595,11 +2597,11 @@
       <c r="F77">
         <v>6</v>
       </c>
-      <c r="G77">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G77" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2616,13 +2618,13 @@
         <v>-2</v>
       </c>
       <c r="F78">
-        <v>2</v>
-      </c>
-      <c r="G78">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G78" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2639,13 +2641,13 @@
         <v>2</v>
       </c>
       <c r="F79">
-        <v>5</v>
-      </c>
-      <c r="G79">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G79" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2662,13 +2664,13 @@
         <v>-2</v>
       </c>
       <c r="F80">
-        <v>3</v>
-      </c>
-      <c r="G80">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G80" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2685,13 +2687,13 @@
         <v>4</v>
       </c>
       <c r="F81">
-        <v>5</v>
-      </c>
-      <c r="G81">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G81" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2708,13 +2710,13 @@
         <v>-2</v>
       </c>
       <c r="F82">
-        <v>1</v>
-      </c>
-      <c r="G82">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G82" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2731,13 +2733,13 @@
         <v>2</v>
       </c>
       <c r="F83">
-        <v>10</v>
-      </c>
-      <c r="G83">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G83" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2754,13 +2756,13 @@
         <v>4</v>
       </c>
       <c r="F84">
-        <v>1</v>
-      </c>
-      <c r="G84">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G84" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2779,11 +2781,11 @@
       <c r="F85">
         <v>4</v>
       </c>
-      <c r="G85">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G85" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2802,11 +2804,11 @@
       <c r="F86">
         <v>4</v>
       </c>
-      <c r="G86">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G86" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2825,11 +2827,11 @@
       <c r="F87">
         <v>2</v>
       </c>
-      <c r="G87">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G87" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2848,11 +2850,11 @@
       <c r="F88">
         <v>2</v>
       </c>
-      <c r="G88" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G88" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2869,13 +2871,13 @@
         <v>5</v>
       </c>
       <c r="F89">
-        <v>1</v>
-      </c>
-      <c r="G89">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G89" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2894,11 +2896,11 @@
       <c r="F90">
         <v>4</v>
       </c>
-      <c r="G90">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G90" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2917,11 +2919,11 @@
       <c r="F91">
         <v>2</v>
       </c>
-      <c r="G91">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G91" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2931,20 +2933,20 @@
       <c r="C92" t="s">
         <v>55</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D92" s="2" t="s">
         <v>100</v>
       </c>
       <c r="E92">
         <v>2</v>
       </c>
-      <c r="F92">
-        <v>7</v>
-      </c>
-      <c r="G92">
+      <c r="F92" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G92" s="4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2961,13 +2963,13 @@
         <v>-1</v>
       </c>
       <c r="F93">
-        <v>3</v>
-      </c>
-      <c r="G93">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G93" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2984,13 +2986,13 @@
         <v>-1</v>
       </c>
       <c r="F94">
-        <v>1</v>
-      </c>
-      <c r="G94">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G94" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3007,13 +3009,13 @@
         <v>-1</v>
       </c>
       <c r="F95">
-        <v>3</v>
-      </c>
-      <c r="G95">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G95" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3030,13 +3032,13 @@
         <v>-1</v>
       </c>
       <c r="F96">
-        <v>3</v>
-      </c>
-      <c r="G96">
         <v>5</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G96" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3053,13 +3055,13 @@
         <v>2</v>
       </c>
       <c r="F97">
-        <v>5</v>
-      </c>
-      <c r="G97">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G97" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3076,13 +3078,13 @@
         <v>2</v>
       </c>
       <c r="F98">
-        <v>7</v>
-      </c>
-      <c r="G98">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G98" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3099,13 +3101,13 @@
         <v>-2</v>
       </c>
       <c r="F99">
-        <v>2</v>
-      </c>
-      <c r="G99">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G99" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3122,13 +3124,13 @@
         <v>6</v>
       </c>
       <c r="F100">
-        <v>1</v>
-      </c>
-      <c r="G100">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G100" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3138,20 +3140,20 @@
       <c r="C101" t="s">
         <v>75</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D101" s="2" t="s">
         <v>113</v>
       </c>
       <c r="E101">
         <v>3</v>
       </c>
-      <c r="F101">
-        <v>7</v>
-      </c>
-      <c r="G101" s="2">
+      <c r="F101" s="2">
+        <v>10</v>
+      </c>
+      <c r="G101" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3168,13 +3170,13 @@
         <v>-2</v>
       </c>
       <c r="F102">
-        <v>2</v>
-      </c>
-      <c r="G102">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G102" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3191,13 +3193,13 @@
         <v>-2</v>
       </c>
       <c r="F103">
-        <v>2</v>
-      </c>
-      <c r="G103">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G103" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3214,13 +3216,13 @@
         <v>-2</v>
       </c>
       <c r="F104">
-        <v>1</v>
-      </c>
-      <c r="G104">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G104" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3237,13 +3239,13 @@
         <v>-2</v>
       </c>
       <c r="F105">
-        <v>2</v>
-      </c>
-      <c r="G105">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G105" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3262,11 +3264,11 @@
       <c r="F106">
         <v>4</v>
       </c>
-      <c r="G106">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G106" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3283,13 +3285,13 @@
         <v>3</v>
       </c>
       <c r="F107">
-        <v>5</v>
-      </c>
-      <c r="G107">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G107" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3308,11 +3310,11 @@
       <c r="F108">
         <v>2</v>
       </c>
-      <c r="G108">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G108" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3329,13 +3331,13 @@
         <v>-2</v>
       </c>
       <c r="F109">
-        <v>1</v>
-      </c>
-      <c r="G109">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G109" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3354,11 +3356,11 @@
       <c r="F110">
         <v>4</v>
       </c>
-      <c r="G110">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G110" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3375,13 +3377,13 @@
         <v>2</v>
       </c>
       <c r="F111">
-        <v>5</v>
-      </c>
-      <c r="G111">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G111" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3400,11 +3402,11 @@
       <c r="F112">
         <v>3</v>
       </c>
-      <c r="G112">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G112" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3421,13 +3423,13 @@
         <v>-2</v>
       </c>
       <c r="F113">
-        <v>2</v>
-      </c>
-      <c r="G113">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G113" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3444,13 +3446,13 @@
         <v>6</v>
       </c>
       <c r="F114">
-        <v>1</v>
-      </c>
-      <c r="G114">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G114" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3469,11 +3471,11 @@
       <c r="F115">
         <v>4</v>
       </c>
-      <c r="G115">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G115" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3492,11 +3494,11 @@
       <c r="F116">
         <v>2</v>
       </c>
-      <c r="G116">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G116" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3515,11 +3517,11 @@
       <c r="F117">
         <v>2</v>
       </c>
-      <c r="G117">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G117" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3538,11 +3540,11 @@
       <c r="F118">
         <v>4</v>
       </c>
-      <c r="G118">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G118" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3559,13 +3561,13 @@
         <v>2</v>
       </c>
       <c r="F119">
-        <v>1</v>
-      </c>
-      <c r="G119">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G119" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3582,13 +3584,13 @@
         <v>-2</v>
       </c>
       <c r="F120">
-        <v>2</v>
-      </c>
-      <c r="G120">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G120" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3605,13 +3607,13 @@
         <v>-2</v>
       </c>
       <c r="F121">
-        <v>1</v>
-      </c>
-      <c r="G121">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G121" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3628,13 +3630,13 @@
         <v>6</v>
       </c>
       <c r="F122">
-        <v>5</v>
-      </c>
-      <c r="G122">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G122" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3651,13 +3653,13 @@
         <v>2</v>
       </c>
       <c r="F123">
-        <v>5</v>
-      </c>
-      <c r="G123">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G123" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3674,13 +3676,13 @@
         <v>2</v>
       </c>
       <c r="F124">
-        <v>5</v>
-      </c>
-      <c r="G124">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G124" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3697,13 +3699,13 @@
         <v>6</v>
       </c>
       <c r="F125">
-        <v>3</v>
-      </c>
-      <c r="G125">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G125" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3720,13 +3722,13 @@
         <v>6</v>
       </c>
       <c r="F126">
-        <v>3</v>
-      </c>
-      <c r="G126">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G126" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3743,13 +3745,13 @@
         <v>-2</v>
       </c>
       <c r="F127">
-        <v>3</v>
-      </c>
-      <c r="G127">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G127" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3766,13 +3768,13 @@
         <v>-2</v>
       </c>
       <c r="F128">
-        <v>1</v>
-      </c>
-      <c r="G128">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G128" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3789,13 +3791,13 @@
         <v>-2</v>
       </c>
       <c r="F129">
-        <v>1</v>
-      </c>
-      <c r="G129">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G129" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3812,13 +3814,13 @@
         <v>-2</v>
       </c>
       <c r="F130">
-        <v>2</v>
-      </c>
-      <c r="G130">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G130" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3835,13 +3837,13 @@
         <v>-2</v>
       </c>
       <c r="F131">
-        <v>1</v>
-      </c>
-      <c r="G131">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G131" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3858,13 +3860,13 @@
         <v>5</v>
       </c>
       <c r="F132">
-        <v>5</v>
-      </c>
-      <c r="G132">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G132" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3881,13 +3883,13 @@
         <v>-2</v>
       </c>
       <c r="F133">
-        <v>2</v>
-      </c>
-      <c r="G133">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G133" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3904,13 +3906,13 @@
         <v>-2</v>
       </c>
       <c r="F134">
-        <v>1</v>
-      </c>
-      <c r="G134">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G134" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3929,11 +3931,11 @@
       <c r="F135">
         <v>3</v>
       </c>
-      <c r="G135">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G135" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3952,11 +3954,11 @@
       <c r="F136">
         <v>2</v>
       </c>
-      <c r="G136" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G136" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -3966,20 +3968,20 @@
       <c r="C137" t="s">
         <v>87</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D137" s="2" t="s">
         <v>122</v>
       </c>
       <c r="E137">
         <v>3</v>
       </c>
       <c r="F137">
-        <v>4</v>
-      </c>
-      <c r="G137" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G137" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -3996,13 +3998,13 @@
         <v>3</v>
       </c>
       <c r="F138">
-        <v>5</v>
-      </c>
-      <c r="G138">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G138" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4021,11 +4023,11 @@
       <c r="F139">
         <v>2</v>
       </c>
-      <c r="G139">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G139" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4042,13 +4044,13 @@
         <v>-1</v>
       </c>
       <c r="F140">
-        <v>3</v>
-      </c>
-      <c r="G140">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G140" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4067,11 +4069,11 @@
       <c r="F141">
         <v>8</v>
       </c>
-      <c r="G141">
+      <c r="G141" s="4">
         <v>8</v>
       </c>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4088,13 +4090,13 @@
         <v>-2</v>
       </c>
       <c r="F142">
-        <v>1</v>
-      </c>
-      <c r="G142">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G142" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4111,13 +4113,13 @@
         <v>-2</v>
       </c>
       <c r="F143">
-        <v>2</v>
-      </c>
-      <c r="G143">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G143" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4136,11 +4138,11 @@
       <c r="F144">
         <v>2</v>
       </c>
-      <c r="G144">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G144" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4157,13 +4159,13 @@
         <v>6</v>
       </c>
       <c r="F145">
-        <v>1</v>
-      </c>
-      <c r="G145">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G145" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4180,13 +4182,13 @@
         <v>2</v>
       </c>
       <c r="F146">
-        <v>4</v>
-      </c>
-      <c r="G146">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G146" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4205,11 +4207,11 @@
       <c r="F147">
         <v>3</v>
       </c>
-      <c r="G147">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G147" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4228,11 +4230,11 @@
       <c r="F148">
         <v>4</v>
       </c>
-      <c r="G148">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G148" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4249,13 +4251,14 @@
         <v>4</v>
       </c>
       <c r="F149">
-        <v>1</v>
-      </c>
-      <c r="G149">
+        <v>8</v>
+      </c>
+      <c r="G149" s="4">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>